<commit_message>
added classses for Invoice Factory
</commit_message>
<xml_diff>
--- a/src/testData/TestData.xlsx
+++ b/src/testData/TestData.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t xml:space="preserve">Test Case Name</t>
   </si>
@@ -37,23 +38,102 @@
     <t xml:space="preserve">APACHE_POI_TC</t>
   </si>
   <si>
-    <t xml:space="preserve">sima77</t>
-  </si>
-  <si>
-    <t xml:space="preserve">itbootcamp</t>
-  </si>
-  <si>
-    <t>Pass</t>
+    <t xml:space="preserve">quadrum.miroslava@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qwe123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCaseName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClientName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ContactName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RegistryNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DateAdded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgreementDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestResult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AddNewClientTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jagoda PR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jagoda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jp@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12332</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serbia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beograd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-1–29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -78,6 +158,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -125,7 +212,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -135,6 +222,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -157,16 +252,18 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="16.17" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="10.43" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="9.78" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.49"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -187,17 +284,20 @@
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="quadrum.miroslava@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -206,4 +306,128 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="14.01"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="3" t="n">
+        <v>11000</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="jp@gmail.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>